<commit_message>
bug fix - kfold working
</commit_message>
<xml_diff>
--- a/checkpoints/model_metrics.xlsx
+++ b/checkpoints/model_metrics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t xml:space="preserve">Solubility</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t xml:space="preserve">roc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stdev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_roc</t>
   </si>
   <si>
     <t xml:space="preserve">RDKIT RF</t>
@@ -95,11 +104,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -120,6 +130,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,12 +181,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,10 +211,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -308,6 +329,18 @@
       <c r="I21" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="J21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -361,10 +394,26 @@
       <c r="I24" s="0" t="n">
         <v>0.724998855311355</v>
       </c>
+      <c r="J24" s="2" t="n">
+        <f aca="false">AVERAGE(H24,F24,D24)</f>
+        <v>0.768333333333333</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <f aca="false">STDEV(H24,F24,D24)</f>
+        <v>0.00416333199893227</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <f aca="false">AVERAGE(I24,G24,E24)</f>
+        <v>0.726763583638584</v>
+      </c>
+      <c r="M24" s="2" t="n">
+        <f aca="false">STDEV(I24,G24,E24)</f>
+        <v>0.00284805627669748</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>1.28000000119209</v>
@@ -387,10 +436,26 @@
       <c r="I25" s="0" t="n">
         <v>0.7255370497558</v>
       </c>
+      <c r="J25" s="2" t="n">
+        <f aca="false">AVERAGE(H25,F25,D25)</f>
+        <v>0.762666666666667</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <f aca="false">STDEV(H25,F25,D25)</f>
+        <v>0.00251661147842354</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <f aca="false">AVERAGE(I25,G25,E25)</f>
+        <v>0.725086106023606</v>
+      </c>
+      <c r="M25" s="2" t="n">
+        <f aca="false">STDEV(I25,G25,E25)</f>
+        <v>0.0029244490117117</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>1.26499998569489</v>
@@ -413,10 +478,26 @@
       <c r="I26" s="0" t="n">
         <v>0.721227297008547</v>
       </c>
+      <c r="J26" s="2" t="n">
+        <f aca="false">AVERAGE(H26,F26,D26)</f>
+        <v>0.759666666666667</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <f aca="false">STDEV(H26,F26,D26)</f>
+        <v>0.000577350269189626</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <f aca="false">AVERAGE(I26,G26,E26)</f>
+        <v>0.720372468966219</v>
+      </c>
+      <c r="M26" s="2" t="n">
+        <f aca="false">STDEV(I26,G26,E26)</f>
+        <v>0.000893891091881286</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">1-D27</f>
@@ -440,10 +521,26 @@
       <c r="I27" s="0" t="n">
         <v>0.704571695665446</v>
       </c>
+      <c r="J27" s="2" t="n">
+        <f aca="false">AVERAGE(H27,F27,D27)</f>
+        <v>0.751666666666667</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <f aca="false">STDEV(H27,F27,D27)</f>
+        <v>0.000577350269189562</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <f aca="false">AVERAGE(I27,G27,E27)</f>
+        <v>0.70303387006512</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <f aca="false">STDEV(I27,G27,E27)</f>
+        <v>0.00165613631895188</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2.28000000119209</v>
@@ -466,10 +563,26 @@
       <c r="I28" s="0" t="n">
         <v>0.694745306776557</v>
       </c>
+      <c r="J28" s="2" t="n">
+        <f aca="false">AVERAGE(H28,F28,D28)</f>
+        <v>0.732666666666667</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <f aca="false">STDEV(H28,F28,D28)</f>
+        <v>0.000577350269189594</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <f aca="false">AVERAGE(I28,G28,E28)</f>
+        <v>0.694054550773301</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <f aca="false">STDEV(I28,G28,E28)</f>
+        <v>0.000645632395819415</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2.26499998569489</v>
@@ -492,10 +605,26 @@
       <c r="I29" s="0" t="n">
         <v>0.701797733516484</v>
       </c>
+      <c r="J29" s="2" t="n">
+        <f aca="false">AVERAGE(H29,F29,D29)</f>
+        <v>0.733333333333333</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <f aca="false">STDEV(H29,F29,D29)</f>
+        <v>0.00208166599946615</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <f aca="false">AVERAGE(I29,G29,E29)</f>
+        <v>0.700885035103785</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <f aca="false">STDEV(I29,G29,E29)</f>
+        <v>0.00172267845853446</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">1-D30</f>
@@ -518,6 +647,22 @@
       </c>
       <c r="I30" s="0" t="n">
         <v>0.707660828754579</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <f aca="false">AVERAGE(H30,F30,D30)</f>
+        <v>0.745666666666667</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <f aca="false">STDEV(H30,F30,D30)</f>
+        <v>0.00873689494805407</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <f aca="false">AVERAGE(I30,G30,E30)</f>
+        <v>0.701071364977615</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <f aca="false">STDEV(I30,G30,E30)</f>
+        <v>0.00963044305193099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compare reg add best metrics sol
</commit_message>
<xml_diff>
--- a/checkpoints/model_metrics.xlsx
+++ b/checkpoints/model_metrics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t xml:space="preserve">Solubility</t>
   </si>
@@ -43,22 +43,31 @@
     <t xml:space="preserve">mae</t>
   </si>
   <si>
-    <t xml:space="preserve">Kfold</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resnet18 + Augs</t>
   </si>
   <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resnet18</t>
   </si>
   <si>
     <t xml:space="preserve">Mordred RF</t>
   </si>
   <si>
-    <t xml:space="preserve">Mordred NN</t>
+    <t xml:space="preserve">RDKIT RF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mol2Vec RF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecfp RF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pubchem RF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maccs key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spectrophore</t>
   </si>
   <si>
     <t xml:space="preserve">Cocrystal</t>
@@ -80,24 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">mean_roc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RDKIT RF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mol2Vec RF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ecfp RF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pubchem RF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maccs key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spectrophore</t>
   </si>
 </sst>
 </file>
@@ -211,10 +202,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,20 +243,38 @@
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.248714566230774</v>
@@ -282,23 +291,81 @@
       <c r="F4" s="0" t="n">
         <v>0.182246074080467</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.821875364512533</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.93363946285174</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.965841640884103</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.609196229486432</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.821720294387933</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.934424643127384</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.96626140041123</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.609728853729244</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.821728229549132</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.934405591064197</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.966242173125073</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0.609520694448872</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,42 +376,42 @@
         <v>2</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -353,24 +420,18 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>0.479781568050384</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>0.189999997615814</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1" t="n">
-        <v>0.810000002384186</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>0.861164736164736</v>
-      </c>
+        <v>0.753999984264374</v>
+      </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">1-D24</f>
@@ -413,7 +474,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>1.28000000119209</v>
@@ -455,7 +516,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>1.26499998569489</v>
@@ -497,7 +558,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">1-D27</f>
@@ -540,7 +601,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2.28000000119209</v>
@@ -582,7 +643,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2.26499998569489</v>
@@ -624,7 +685,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">1-D30</f>

</xml_diff>

<commit_message>
fix breaking desc gens
</commit_message>
<xml_diff>
--- a/checkpoints/model_metrics.xlsx
+++ b/checkpoints/model_metrics.xlsx
@@ -20,17 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">Solubility</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">Sol</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
   </si>
   <si>
-    <t xml:space="preserve">val loss</t>
-  </si>
-  <si>
     <t xml:space="preserve">r2 score</t>
   </si>
   <si>
@@ -70,7 +67,7 @@
     <t xml:space="preserve">spectrophore</t>
   </si>
   <si>
-    <t xml:space="preserve">Cocrystal</t>
+    <t xml:space="preserve">CC</t>
   </si>
   <si>
     <t xml:space="preserve">error rate</t>
@@ -100,7 +97,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -121,6 +118,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -172,8 +176,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,7 +189,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,20 +210,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,7 +248,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>3</v>
@@ -252,7 +260,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>3</v>
@@ -263,109 +271,247 @@
       <c r="M2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.248714566230774</v>
+        <v>0.783726169762395</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.95228410776943</v>
+        <v>1.13111340999603</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.248714566230774</v>
+        <v>1.06300181150436</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0.498712927103043</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0.182246074080467</v>
+        <v>0.693051016330719</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.821875364512533</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.821875364512533</v>
+        <v>0.93363946285174</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.93363946285174</v>
+        <v>0.965841640884103</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0.965841640884103</v>
+        <v>0.609196229486432</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.609196229486432</v>
+        <v>0.821720294387933</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.821720294387933</v>
+        <v>0.934424643127384</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0.934424643127384</v>
+        <v>0.96626140041123</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.96626140041123</v>
+        <v>0.609728853729244</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.609728853729244</v>
+        <v>0.821728229549132</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0.821728229549132</v>
+        <v>0.934405591064197</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0.934405591064197</v>
+        <v>0.966242173125073</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>0.966242173125073</v>
-      </c>
-      <c r="N5" s="0" t="n">
         <v>0.609520694448872</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.773747945998141</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1.18605159452109</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1.08849805826094</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.72734547120797</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.773551999684163</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1.18710416117267</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1.08895938051468</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.727413061012078</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.77412330032003</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1.18408854624062</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1.08759383338173</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0.726949552567496</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.698163970262569</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1.58195465086144</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1.25725807907887</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.833168206747544</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.698084195847153</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1.58233787378358</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1.25741883578082</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.832624288518198</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.698010740997796</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>1.58269775449524</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>1.25756993747823</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0.833259546086923</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.72025260687738</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1.4657662771765</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1.21032508263807</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.798652426595308</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.720445494766854</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1.46479781646264</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1.20992255221951</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.79850540223485</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.720611722424659</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1.46394201669567</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>1.2095553766259</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>0.798120062854116</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>15</v>
+      <c r="B11" s="1" t="n">
+        <v>0.610624970744845</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>2.01977947981916</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1.42090215566551</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>1.00957964435492</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0.61074170663389</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>2.01905111238678</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1.42067312565769</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>1.00960260092972</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>0.61042119385788</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>2.02075787663089</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>1.42126949501312</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>1.0102269957577</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>17</v>
@@ -382,13 +528,13 @@
         <v>18</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>18</v>
@@ -403,326 +549,323 @@
         <v>21</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="n">
-        <v>0.753999984264374</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="n">
+        <v>0.820999985933304</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0.839042983058608</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">1-C24</f>
+        <v>0.227</v>
       </c>
       <c r="C24" s="0" t="n">
-        <f aca="false">1-D24</f>
-        <v>0.227</v>
-      </c>
-      <c r="D24" s="0" t="n">
         <v>0.773</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="D24" s="2" t="n">
         <v>0.730049221611722</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>0.767</v>
+      </c>
       <c r="F24" s="0" t="n">
-        <v>0.767</v>
+        <v>0.725242673992674</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.725242673992674</v>
+        <v>0.765</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>0.765</v>
-      </c>
-      <c r="I24" s="0" t="n">
         <v>0.724998855311355</v>
       </c>
-      <c r="J24" s="2" t="n">
+      <c r="I24" s="3" t="n">
+        <f aca="false">AVERAGE(G24,E24,C24)</f>
+        <v>0.768333333333333</v>
+      </c>
+      <c r="J24" s="3" t="n">
+        <f aca="false">STDEV(G24,E24,C24)</f>
+        <v>0.00416333199893227</v>
+      </c>
+      <c r="K24" s="3" t="n">
         <f aca="false">AVERAGE(H24,F24,D24)</f>
-        <v>0.768333333333333</v>
-      </c>
-      <c r="K24" s="2" t="n">
+        <v>0.726763583638584</v>
+      </c>
+      <c r="L24" s="3" t="n">
         <f aca="false">STDEV(H24,F24,D24)</f>
-        <v>0.00416333199893227</v>
-      </c>
-      <c r="L24" s="2" t="n">
-        <f aca="false">AVERAGE(I24,G24,E24)</f>
-        <v>0.726763583638584</v>
-      </c>
-      <c r="M24" s="2" t="n">
-        <f aca="false">STDEV(I24,G24,E24)</f>
         <v>0.00284805627669748</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="2" t="n">
         <v>1.28000000119209</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="C25" s="0" t="n">
         <v>0.76</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="D25" s="2" t="n">
         <v>0.721962377899878</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>0.765</v>
+      </c>
       <c r="F25" s="0" t="n">
-        <v>0.765</v>
+        <v>0.72775889041514</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0.72775889041514</v>
+        <v>0.763</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>0.763</v>
-      </c>
-      <c r="I25" s="0" t="n">
         <v>0.7255370497558</v>
       </c>
-      <c r="J25" s="2" t="n">
+      <c r="I25" s="3" t="n">
+        <f aca="false">AVERAGE(G25,E25,C25)</f>
+        <v>0.762666666666667</v>
+      </c>
+      <c r="J25" s="3" t="n">
+        <f aca="false">STDEV(G25,E25,C25)</f>
+        <v>0.00251661147842354</v>
+      </c>
+      <c r="K25" s="3" t="n">
         <f aca="false">AVERAGE(H25,F25,D25)</f>
-        <v>0.762666666666667</v>
-      </c>
-      <c r="K25" s="2" t="n">
+        <v>0.725086106023606</v>
+      </c>
+      <c r="L25" s="3" t="n">
         <f aca="false">STDEV(H25,F25,D25)</f>
-        <v>0.00251661147842354</v>
-      </c>
-      <c r="L25" s="2" t="n">
-        <f aca="false">AVERAGE(I25,G25,E25)</f>
-        <v>0.725086106023606</v>
-      </c>
-      <c r="M25" s="2" t="n">
-        <f aca="false">STDEV(I25,G25,E25)</f>
         <v>0.0029244490117117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2" t="n">
         <v>1.26499998569489</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="C26" s="0" t="n">
         <v>0.76</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="D26" s="2" t="n">
         <v>0.719444062881563</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>0.759</v>
+      </c>
       <c r="F26" s="0" t="n">
-        <v>0.759</v>
+        <v>0.720446047008547</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.720446047008547</v>
+        <v>0.76</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="I26" s="0" t="n">
         <v>0.721227297008547</v>
       </c>
-      <c r="J26" s="2" t="n">
+      <c r="I26" s="3" t="n">
+        <f aca="false">AVERAGE(G26,E26,C26)</f>
+        <v>0.759666666666667</v>
+      </c>
+      <c r="J26" s="3" t="n">
+        <f aca="false">STDEV(G26,E26,C26)</f>
+        <v>0.000577350269189626</v>
+      </c>
+      <c r="K26" s="3" t="n">
         <f aca="false">AVERAGE(H26,F26,D26)</f>
-        <v>0.759666666666667</v>
-      </c>
-      <c r="K26" s="2" t="n">
+        <v>0.720372468966219</v>
+      </c>
+      <c r="L26" s="3" t="n">
         <f aca="false">STDEV(H26,F26,D26)</f>
-        <v>0.000577350269189626</v>
-      </c>
-      <c r="L26" s="2" t="n">
-        <f aca="false">AVERAGE(I26,G26,E26)</f>
-        <v>0.720372468966219</v>
-      </c>
-      <c r="M26" s="2" t="n">
-        <f aca="false">STDEV(I26,G26,E26)</f>
         <v>0.000893891091881286</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">1-C27</f>
+        <v>0.248</v>
       </c>
       <c r="C27" s="0" t="n">
-        <f aca="false">1-D27</f>
-        <v>0.248</v>
-      </c>
-      <c r="D27" s="0" t="n">
         <v>0.752</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="D27" s="2" t="n">
         <v>0.703249389499389</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>0.751</v>
+      </c>
       <c r="F27" s="0" t="n">
-        <v>0.751</v>
+        <v>0.701280525030525</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.701280525030525</v>
+        <v>0.752</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>0.752</v>
-      </c>
-      <c r="I27" s="0" t="n">
         <v>0.704571695665446</v>
       </c>
-      <c r="J27" s="2" t="n">
+      <c r="I27" s="3" t="n">
+        <f aca="false">AVERAGE(G27,E27,C27)</f>
+        <v>0.751666666666667</v>
+      </c>
+      <c r="J27" s="3" t="n">
+        <f aca="false">STDEV(G27,E27,C27)</f>
+        <v>0.000577350269189562</v>
+      </c>
+      <c r="K27" s="3" t="n">
         <f aca="false">AVERAGE(H27,F27,D27)</f>
-        <v>0.751666666666667</v>
-      </c>
-      <c r="K27" s="2" t="n">
+        <v>0.70303387006512</v>
+      </c>
+      <c r="L27" s="3" t="n">
         <f aca="false">STDEV(H27,F27,D27)</f>
-        <v>0.000577350269189562</v>
-      </c>
-      <c r="L27" s="2" t="n">
-        <f aca="false">AVERAGE(I27,G27,E27)</f>
-        <v>0.70303387006512</v>
-      </c>
-      <c r="M27" s="2" t="n">
-        <f aca="false">STDEV(I27,G27,E27)</f>
         <v>0.00165613631895188</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B28" s="2" t="n">
         <v>2.28000000119209</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="C28" s="2" t="n">
         <v>0.733</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="D28" s="2" t="n">
         <v>0.693466307997558</v>
       </c>
+      <c r="E28" s="0" t="n">
+        <v>0.732</v>
+      </c>
       <c r="F28" s="0" t="n">
-        <v>0.732</v>
+        <v>0.693952037545788</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0.693952037545788</v>
+        <v>0.733</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>0.733</v>
-      </c>
-      <c r="I28" s="0" t="n">
         <v>0.694745306776557</v>
       </c>
-      <c r="J28" s="2" t="n">
+      <c r="I28" s="3" t="n">
+        <f aca="false">AVERAGE(G28,E28,C28)</f>
+        <v>0.732666666666667</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <f aca="false">STDEV(G28,E28,C28)</f>
+        <v>0.000577350269189594</v>
+      </c>
+      <c r="K28" s="3" t="n">
         <f aca="false">AVERAGE(H28,F28,D28)</f>
-        <v>0.732666666666667</v>
-      </c>
-      <c r="K28" s="2" t="n">
+        <v>0.694054550773301</v>
+      </c>
+      <c r="L28" s="3" t="n">
         <f aca="false">STDEV(H28,F28,D28)</f>
-        <v>0.000577350269189594</v>
-      </c>
-      <c r="L28" s="2" t="n">
-        <f aca="false">AVERAGE(I28,G28,E28)</f>
-        <v>0.694054550773301</v>
-      </c>
-      <c r="M28" s="2" t="n">
-        <f aca="false">STDEV(I28,G28,E28)</f>
         <v>0.000645632395819415</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2" t="n">
         <v>2.26499998569489</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="C29" s="0" t="n">
         <v>0.735</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="D29" s="2" t="n">
         <v>0.701959325396826</v>
       </c>
+      <c r="E29" s="0" t="n">
+        <v>0.731</v>
+      </c>
       <c r="F29" s="0" t="n">
-        <v>0.731</v>
+        <v>0.698898046398046</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.698898046398046</v>
+        <v>0.734</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>0.734</v>
-      </c>
-      <c r="I29" s="0" t="n">
         <v>0.701797733516484</v>
       </c>
-      <c r="J29" s="2" t="n">
+      <c r="I29" s="3" t="n">
+        <f aca="false">AVERAGE(G29,E29,C29)</f>
+        <v>0.733333333333333</v>
+      </c>
+      <c r="J29" s="3" t="n">
+        <f aca="false">STDEV(G29,E29,C29)</f>
+        <v>0.00208166599946615</v>
+      </c>
+      <c r="K29" s="3" t="n">
         <f aca="false">AVERAGE(H29,F29,D29)</f>
-        <v>0.733333333333333</v>
-      </c>
-      <c r="K29" s="2" t="n">
+        <v>0.700885035103785</v>
+      </c>
+      <c r="L29" s="3" t="n">
         <f aca="false">STDEV(H29,F29,D29)</f>
-        <v>0.00208166599946615</v>
-      </c>
-      <c r="L29" s="2" t="n">
-        <f aca="false">AVERAGE(I29,G29,E29)</f>
-        <v>0.700885035103785</v>
-      </c>
-      <c r="M29" s="2" t="n">
-        <f aca="false">STDEV(I29,G29,E29)</f>
         <v>0.00172267845853446</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">1-C30</f>
+        <v>0.264</v>
       </c>
       <c r="C30" s="0" t="n">
-        <f aca="false">1-D30</f>
-        <v>0.264</v>
-      </c>
-      <c r="D30" s="0" t="n">
         <v>0.736</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="D30" s="2" t="n">
         <v>0.690019078144078</v>
       </c>
+      <c r="E30" s="0" t="n">
+        <v>0.748</v>
+      </c>
       <c r="F30" s="0" t="n">
-        <v>0.748</v>
+        <v>0.705534188034188</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.705534188034188</v>
+        <v>0.753</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>0.753</v>
-      </c>
-      <c r="I30" s="0" t="n">
         <v>0.707660828754579</v>
       </c>
-      <c r="J30" s="2" t="n">
+      <c r="I30" s="3" t="n">
+        <f aca="false">AVERAGE(G30,E30,C30)</f>
+        <v>0.745666666666667</v>
+      </c>
+      <c r="J30" s="3" t="n">
+        <f aca="false">STDEV(G30,E30,C30)</f>
+        <v>0.00873689494805407</v>
+      </c>
+      <c r="K30" s="3" t="n">
         <f aca="false">AVERAGE(H30,F30,D30)</f>
-        <v>0.745666666666667</v>
-      </c>
-      <c r="K30" s="2" t="n">
+        <v>0.701071364977615</v>
+      </c>
+      <c r="L30" s="3" t="n">
         <f aca="false">STDEV(H30,F30,D30)</f>
-        <v>0.00873689494805407</v>
-      </c>
-      <c r="L30" s="2" t="n">
-        <f aca="false">AVERAGE(I30,G30,E30)</f>
-        <v>0.701071364977615</v>
-      </c>
-      <c r="M30" s="2" t="n">
-        <f aca="false">STDEV(I30,G30,E30)</f>
         <v>0.00963044305193099</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove specified random seeding
</commit_message>
<xml_diff>
--- a/checkpoints/model_metrics.xlsx
+++ b/checkpoints/model_metrics.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
   <si>
     <t xml:space="preserve">Sol</t>
   </si>
@@ -83,6 +84,12 @@
   </si>
   <si>
     <t xml:space="preserve">mean_roc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rand seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed seed in this </t>
   </si>
 </sst>
 </file>
@@ -94,7 +101,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -126,6 +133,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -173,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -187,6 +202,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,8 +232,8 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -274,58 +297,46 @@
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0.783726169762395</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1.13111340999603</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1.06300181150436</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0.693051016330719</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.821875364512533</v>
+        <v>0.821280522001387</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.93363946285174</v>
+        <v>0.936387891083399</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.965841640884103</v>
+        <v>0.966794435039716</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0.609196229486432</v>
+        <v>0.6095322828548</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.821720294387933</v>
+        <v>0.82061389144013</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.934424643127384</v>
+        <v>0.940697642661704</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0.96626140041123</v>
+        <v>0.968949824673278</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.609728853729244</v>
+        <v>0.610706692748174</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.821728229549132</v>
+        <v>0.821518042794237</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0.934405591064197</v>
+        <v>0.935286993608807</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0.966242173125073</v>
+        <v>0.966748024380555</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>0.609520694448872</v>
+        <v>0.609503378119049</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,40 +344,40 @@
         <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.819432735566018</v>
+        <v>0.818494764267101</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.946423736293863</v>
+        <v>0.951289001197056</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.972403231598438</v>
+        <v>0.974870481137826</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0.610709269446693</v>
+        <v>0.613274896713269</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.819760935322595</v>
+        <v>0.8174165617867</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.944668571606909</v>
+        <v>0.955642324964783</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>0.971516897621851</v>
+        <v>0.977096979129114</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.610886797104358</v>
+        <v>0.612213171235938</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.819605034142445</v>
+        <v>0.817963514638863</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>0.945530460918191</v>
+        <v>0.953774794661632</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0.971933927708493</v>
+        <v>0.976410854915658</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>0.61106196631443</v>
+        <v>0.613449556400731</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,82 +385,46 @@
         <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.773747945998141</v>
+        <v>0.774459655706926</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>1.18605159452109</v>
+        <v>1.18189968033683</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1.08849805826094</v>
+        <v>1.0863917427271</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0.72734547120797</v>
+        <v>0.725621513040646</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.773551999684163</v>
+        <v>0.773828297298869</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1.18710416117267</v>
+        <v>1.18501512906011</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>1.08895938051468</v>
+        <v>1.08752983674279</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0.727413061012078</v>
+        <v>0.726198325033304</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.77412330032003</v>
+        <v>0.774062945896588</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>1.18408854624062</v>
+        <v>1.18438420575572</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>1.08759383338173</v>
+        <v>1.08758110993771</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>0.726949552567496</v>
+        <v>0.726069060651303</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>0.698163970262569</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>1.58195465086144</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>1.25725807907887</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0.833168206747544</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0.698084195847153</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>1.58233787378358</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>1.25741883578082</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>0.832624288518198</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0.698010740997796</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>1.58269775449524</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>1.25756993747823</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>0.833259546086923</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -460,83 +435,11 @@
       <c r="A10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>0.72025260687738</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>1.4657662771765</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>1.21032508263807</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>0.798652426595308</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>0.720445494766854</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>1.46479781646264</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>1.20992255221951</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>0.79850540223485</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>0.720611722424659</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>1.46394201669567</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>1.2095553766259</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>0.798120062854116</v>
-      </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="n">
-        <v>0.610624970744845</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>2.01977947981916</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1.42090215566551</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>1.00957964435492</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>0.61074170663389</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>2.01905111238678</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>1.42067312565769</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>1.00960260092972</v>
-      </c>
-      <c r="J11" s="1" t="n">
-        <v>0.61042119385788</v>
-      </c>
-      <c r="K11" s="1" t="n">
-        <v>2.02075787663089</v>
-      </c>
-      <c r="L11" s="1" t="n">
-        <v>1.42126949501312</v>
-      </c>
-      <c r="M11" s="1" t="n">
-        <v>1.0102269957577</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
@@ -584,44 +487,48 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
+      <c r="H22" s="3" t="e">
+        <f aca="false">AVERAGE(F22,D22,B22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="3" t="e">
+        <f aca="false">STDEV(F22,D22,B22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="3" t="e">
+        <f aca="false">AVERAGE(G22,E22,C22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="3" t="e">
+        <f aca="false">STDEV(G22,E22,C22)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>0.820999985933304</v>
+        <v>0.810999965667725</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.839042983058608</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>0.804999989271164</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>0.834487103174603</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>0.818999981880188</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <v>0.838331015338828</v>
+        <v>0.837458781669719</v>
       </c>
       <c r="H23" s="3" t="n">
         <f aca="false">AVERAGE(F23,D23,B23)</f>
-        <v>0.814999985694885</v>
-      </c>
-      <c r="I23" s="3" t="n">
+        <v>0.810999965667725</v>
+      </c>
+      <c r="I23" s="3" t="e">
         <f aca="false">STDEV(F23,D23,B23)</f>
-        <v>0.00871779504283917</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J23" s="3" t="n">
         <f aca="false">AVERAGE(G23,E23,C23)</f>
-        <v>0.837287033857346</v>
-      </c>
-      <c r="K23" s="3" t="n">
+        <v>0.837458781669719</v>
+      </c>
+      <c r="K23" s="3" t="e">
         <f aca="false">STDEV(G23,E23,C23)</f>
-        <v>0.0024508025990738</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,38 +536,38 @@
         <v>8</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.773</v>
+        <v>0.754</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.730049221611722</v>
+        <v>0.70975351037851</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.767</v>
+        <v>0.768</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>0.725242673992674</v>
+        <v>0.724553762210012</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>0.765</v>
+        <v>0.632122864335497</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.724998855311355</v>
+        <v>0.722599587912088</v>
       </c>
       <c r="H24" s="3" t="n">
         <f aca="false">AVERAGE(F24,D24,B24)</f>
-        <v>0.768333333333333</v>
+        <v>0.718040954778499</v>
       </c>
       <c r="I24" s="3" t="n">
         <f aca="false">STDEV(F24,D24,B24)</f>
-        <v>0.00416333199893227</v>
+        <v>0.074735792623273</v>
       </c>
       <c r="J24" s="3" t="n">
         <f aca="false">AVERAGE(G24,E24,C24)</f>
-        <v>0.726763583638584</v>
+        <v>0.718968953500204</v>
       </c>
       <c r="K24" s="3" t="n">
         <f aca="false">STDEV(G24,E24,C24)</f>
-        <v>0.00284805627669748</v>
+        <v>0.00804039757994205</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,38 +575,41 @@
         <v>9</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.76</v>
+        <v>0.767</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.721962377899878</v>
+        <v>0.728793116605617</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.765</v>
+        <v>0.762</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>0.72775889041514</v>
+        <v>0.721022588522589</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>0.763</v>
+        <v>0.766</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0.7255370497558</v>
+        <v>0.726394993894994</v>
       </c>
       <c r="H25" s="3" t="n">
         <f aca="false">AVERAGE(F25,D25,B25)</f>
-        <v>0.762666666666667</v>
+        <v>0.765</v>
       </c>
       <c r="I25" s="3" t="n">
         <f aca="false">STDEV(F25,D25,B25)</f>
-        <v>0.00251661147842354</v>
+        <v>0.00264575131106459</v>
       </c>
       <c r="J25" s="3" t="n">
         <f aca="false">AVERAGE(G25,E25,C25)</f>
-        <v>0.725086106023606</v>
+        <v>0.725403566341066</v>
       </c>
       <c r="K25" s="3" t="n">
         <f aca="false">STDEV(G25,E25,C25)</f>
-        <v>0.0029244490117117</v>
+        <v>0.00397900403597391</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,38 +617,38 @@
         <v>10</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.76</v>
+        <v>0.761</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.719444062881563</v>
+        <v>0.720924336080586</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.759</v>
+        <v>0.774</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>0.720446047008547</v>
+        <v>0.732605311355311</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0.76</v>
+        <v>0.765</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.721227297008547</v>
+        <v>0.724303456959707</v>
       </c>
       <c r="H26" s="3" t="n">
         <f aca="false">AVERAGE(F26,D26,B26)</f>
-        <v>0.759666666666667</v>
+        <v>0.766666666666667</v>
       </c>
       <c r="I26" s="3" t="n">
         <f aca="false">STDEV(F26,D26,B26)</f>
-        <v>0.000577350269189626</v>
+        <v>0.0066583281184794</v>
       </c>
       <c r="J26" s="3" t="n">
         <f aca="false">AVERAGE(G26,E26,C26)</f>
-        <v>0.720372468966219</v>
+        <v>0.725944368131868</v>
       </c>
       <c r="K26" s="3" t="n">
         <f aca="false">STDEV(G26,E26,C26)</f>
-        <v>0.000893891091881286</v>
+        <v>0.00601088495551016</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,77 +656,77 @@
         <v>11</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.752</v>
+        <v>0.747</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.703249389499389</v>
+        <v>0.697798382173382</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0.751</v>
+        <v>0.747</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>0.701280525030525</v>
+        <v>0.696173878205128</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0.752</v>
+        <v>0.74</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.704571695665446</v>
+        <v>0.690292277167277</v>
       </c>
       <c r="H27" s="3" t="n">
         <f aca="false">AVERAGE(F27,D27,B27)</f>
-        <v>0.751666666666667</v>
+        <v>0.744666666666667</v>
       </c>
       <c r="I27" s="3" t="n">
         <f aca="false">STDEV(F27,D27,B27)</f>
-        <v>0.000577350269189562</v>
+        <v>0.00404145188432742</v>
       </c>
       <c r="J27" s="3" t="n">
         <f aca="false">AVERAGE(G27,E27,C27)</f>
-        <v>0.70303387006512</v>
+        <v>0.694754845848596</v>
       </c>
       <c r="K27" s="3" t="n">
         <f aca="false">STDEV(G27,E27,C27)</f>
-        <v>0.00165613631895188</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+        <v>0.00394913189350936</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="2" t="n">
-        <v>0.733</v>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>0.693466307997558</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>0.732</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>0.693952037545788</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>0.733</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <v>0.694745306776557</v>
-      </c>
-      <c r="H28" s="3" t="n">
+      <c r="B28" s="4" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>0.704304029304029</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>0.72515350877193</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>0.682327233378809</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>0.685876831501832</v>
+      </c>
+      <c r="H28" s="5" t="n">
         <f aca="false">AVERAGE(F28,D28,B28)</f>
-        <v>0.732666666666667</v>
-      </c>
-      <c r="I28" s="3" t="n">
+        <v>0.73071783625731</v>
+      </c>
+      <c r="I28" s="5" t="n">
         <f aca="false">STDEV(F28,D28,B28)</f>
-        <v>0.000577350269189594</v>
-      </c>
-      <c r="J28" s="3" t="n">
+        <v>0.00809143406779152</v>
+      </c>
+      <c r="J28" s="5" t="n">
         <f aca="false">AVERAGE(G28,E28,C28)</f>
-        <v>0.694054550773301</v>
-      </c>
-      <c r="K28" s="3" t="n">
+        <v>0.69083603139489</v>
+      </c>
+      <c r="K28" s="5" t="n">
         <f aca="false">STDEV(G28,E28,C28)</f>
-        <v>0.000645632395819415</v>
+        <v>0.0117978869917107</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,38 +734,38 @@
         <v>13</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>0.735</v>
+        <v>0.716</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.701959325396826</v>
+        <v>0.68074213980464</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>0.731</v>
+        <v>0.724</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>0.698898046398046</v>
+        <v>0.688944978632479</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0.734</v>
+        <v>0.726</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.701797733516484</v>
+        <v>0.690854128510378</v>
       </c>
       <c r="H29" s="3" t="n">
         <f aca="false">AVERAGE(F29,D29,B29)</f>
-        <v>0.733333333333333</v>
+        <v>0.722</v>
       </c>
       <c r="I29" s="3" t="n">
         <f aca="false">STDEV(F29,D29,B29)</f>
-        <v>0.00208166599946615</v>
+        <v>0.00529150262212919</v>
       </c>
       <c r="J29" s="3" t="n">
         <f aca="false">AVERAGE(G29,E29,C29)</f>
-        <v>0.700885035103785</v>
+        <v>0.686847082315832</v>
       </c>
       <c r="K29" s="3" t="n">
         <f aca="false">STDEV(G29,E29,C29)</f>
-        <v>0.00172267845853446</v>
+        <v>0.00537251855397406</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,38 +773,38 @@
         <v>14</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0.736</v>
+        <v>0.738</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0.690019078144078</v>
+        <v>0.738</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.748</v>
+        <v>0.746</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>0.705534188034188</v>
+        <v>0.701095848595849</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0.753</v>
+        <v>0.749</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.707660828754579</v>
+        <v>0.705048458485959</v>
       </c>
       <c r="H30" s="3" t="n">
         <f aca="false">AVERAGE(F30,D30,B30)</f>
-        <v>0.745666666666667</v>
+        <v>0.744333333333333</v>
       </c>
       <c r="I30" s="3" t="n">
         <f aca="false">STDEV(F30,D30,B30)</f>
-        <v>0.00873689494805407</v>
+        <v>0.00568624070307729</v>
       </c>
       <c r="J30" s="3" t="n">
         <f aca="false">AVERAGE(G30,E30,C30)</f>
-        <v>0.701071364977615</v>
+        <v>0.714714769027269</v>
       </c>
       <c r="K30" s="3" t="n">
         <f aca="false">STDEV(G30,E30,C30)</f>
-        <v>0.00963044305193099</v>
+        <v>0.0202622127944093</v>
       </c>
     </row>
   </sheetData>
@@ -906,4 +816,713 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M33" activeCellId="0" sqref="M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.37"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.783726169762395</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1.13111340999603</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1.06300181150436</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.693051016330719</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.821875364512533</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.93363946285174</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.965841640884103</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.609196229486432</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.821720294387933</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.934424643127384</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.96626140041123</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.609728853729244</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.821728229549132</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.934405591064197</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.966242173125073</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.609520694448872</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.819432735566018</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.946423736293863</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.972403231598438</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.610709269446693</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.819760935322595</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.944668571606909</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.971516897621851</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.610886797104358</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.819605034142445</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.945530460918191</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.971933927708493</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0.61106196631443</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.773747945998141</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1.18605159452109</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1.08849805826094</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.72734547120797</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.773551999684163</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1.18710416117267</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1.08895938051468</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.727413061012078</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.77412330032003</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1.18408854624062</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1.08759383338173</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0.726949552567496</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.698163970262569</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1.58195465086144</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1.25725807907887</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.833168206747544</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.698084195847153</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1.58233787378358</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1.25741883578082</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.832624288518198</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.698010740997796</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>1.58269775449524</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>1.25756993747823</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0.833259546086923</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.72025260687738</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1.4657662771765</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1.21032508263807</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.798652426595308</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.720445494766854</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1.46479781646264</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1.20992255221951</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.79850540223485</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.720611722424659</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1.46394201669567</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>1.2095553766259</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>0.798120062854116</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>0.610624970744845</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>2.01977947981916</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1.42090215566551</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>1.00957964435492</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0.61074170663389</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>2.01905111238678</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1.42067312565769</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>1.00960260092972</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>0.61042119385788</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>2.02075787663089</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>1.42126949501312</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>1.0102269957577</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>0.820999985933304</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>0.839042983058608</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0.804999989271164</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.834487103174603</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0.818999981880188</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0.838331015338828</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <f aca="false">AVERAGE(F23,D23,B23)</f>
+        <v>0.814999985694885</v>
+      </c>
+      <c r="I23" s="3" t="n">
+        <f aca="false">STDEV(F23,D23,B23)</f>
+        <v>0.00871779504283917</v>
+      </c>
+      <c r="J23" s="3" t="n">
+        <f aca="false">AVERAGE(G23,E23,C23)</f>
+        <v>0.837287033857346</v>
+      </c>
+      <c r="K23" s="3" t="n">
+        <f aca="false">STDEV(G23,E23,C23)</f>
+        <v>0.0024508025990738</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0.773</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>0.730049221611722</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.725242673992674</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0.724998855311355</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <f aca="false">AVERAGE(F24,D24,B24)</f>
+        <v>0.768333333333333</v>
+      </c>
+      <c r="I24" s="3" t="n">
+        <f aca="false">STDEV(F24,D24,B24)</f>
+        <v>0.00416333199893227</v>
+      </c>
+      <c r="J24" s="3" t="n">
+        <f aca="false">AVERAGE(G24,E24,C24)</f>
+        <v>0.726763583638584</v>
+      </c>
+      <c r="K24" s="3" t="n">
+        <f aca="false">STDEV(G24,E24,C24)</f>
+        <v>0.00284805627669755</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>0.721962377899878</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.72775889041514</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0.763</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0.7255370497558</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <f aca="false">AVERAGE(F25,D25,B25)</f>
+        <v>0.762666666666667</v>
+      </c>
+      <c r="I25" s="3" t="n">
+        <f aca="false">STDEV(F25,D25,B25)</f>
+        <v>0.00251661147842359</v>
+      </c>
+      <c r="J25" s="3" t="n">
+        <f aca="false">AVERAGE(G25,E25,C25)</f>
+        <v>0.725086106023606</v>
+      </c>
+      <c r="K25" s="3" t="n">
+        <f aca="false">STDEV(G25,E25,C25)</f>
+        <v>0.00292444901171158</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>0.719444062881563</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0.759</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.720446047008547</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0.721227297008547</v>
+      </c>
+      <c r="H26" s="3" t="n">
+        <f aca="false">AVERAGE(F26,D26,B26)</f>
+        <v>0.759666666666667</v>
+      </c>
+      <c r="I26" s="3" t="n">
+        <f aca="false">STDEV(F26,D26,B26)</f>
+        <v>0.000577350269189626</v>
+      </c>
+      <c r="J26" s="3" t="n">
+        <f aca="false">AVERAGE(G26,E26,C26)</f>
+        <v>0.720372468966219</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <f aca="false">STDEV(G26,E26,C26)</f>
+        <v>0.000893891091881286</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.752</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0.703249389499389</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0.751</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.701280525030525</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.752</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0.704571695665446</v>
+      </c>
+      <c r="H27" s="3" t="n">
+        <f aca="false">AVERAGE(F27,D27,B27)</f>
+        <v>0.751666666666667</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <f aca="false">STDEV(F27,D27,B27)</f>
+        <v>0.000577350269189626</v>
+      </c>
+      <c r="J27" s="3" t="n">
+        <f aca="false">AVERAGE(G27,E27,C27)</f>
+        <v>0.70303387006512</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <f aca="false">STDEV(G27,E27,C27)</f>
+        <v>0.00165613631895213</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>0.693466307997558</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.732</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.693952037545788</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0.694745306776557</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <f aca="false">AVERAGE(F28,D28,B28)</f>
+        <v>0.732666666666667</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <f aca="false">STDEV(F28,D28,B28)</f>
+        <v>0.000577350269189626</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <f aca="false">AVERAGE(G28,E28,C28)</f>
+        <v>0.694054550773301</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <f aca="false">STDEV(G28,E28,C28)</f>
+        <v>0.000645632395819498</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>0.701959325396826</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0.731</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0.698898046398046</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0.734</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0.701797733516484</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <f aca="false">AVERAGE(F29,D29,B29)</f>
+        <v>0.733333333333333</v>
+      </c>
+      <c r="I29" s="3" t="n">
+        <f aca="false">STDEV(F29,D29,B29)</f>
+        <v>0.00208166599946613</v>
+      </c>
+      <c r="J29" s="3" t="n">
+        <f aca="false">AVERAGE(G29,E29,C29)</f>
+        <v>0.700885035103785</v>
+      </c>
+      <c r="K29" s="3" t="n">
+        <f aca="false">STDEV(G29,E29,C29)</f>
+        <v>0.00172267845853477</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.736</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0.690019078144078</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.748</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0.705534188034188</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0.753</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0.707660828754579</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <f aca="false">AVERAGE(F30,D30,B30)</f>
+        <v>0.745666666666667</v>
+      </c>
+      <c r="I30" s="3" t="n">
+        <f aca="false">STDEV(F30,D30,B30)</f>
+        <v>0.00873689494805411</v>
+      </c>
+      <c r="J30" s="3" t="n">
+        <f aca="false">AVERAGE(G30,E30,C30)</f>
+        <v>0.701071364977615</v>
+      </c>
+      <c r="K30" s="3" t="n">
+        <f aca="false">STDEV(G30,E30,C30)</f>
+        <v>0.0096304430519311</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new metric result added
</commit_message>
<xml_diff>
--- a/checkpoints/model_metrics.xlsx
+++ b/checkpoints/model_metrics.xlsx
@@ -239,10 +239,10 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="0" width="14.74"/>
@@ -685,21 +685,27 @@
       <c r="C22" s="2" t="n">
         <v>0.92961134004884</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>0.904999977350235</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.927132154304029</v>
+      </c>
       <c r="H22" s="3" t="n">
         <f aca="false">AVERAGE(F22,D22,B22)</f>
-        <v>0.900999969244003</v>
-      </c>
-      <c r="I22" s="3" t="e">
+        <v>0.902999973297119</v>
+      </c>
+      <c r="I22" s="3" t="n">
         <f aca="false">STDEV(F22,D22,B22)</f>
-        <v>#DIV/0!</v>
+        <v>0.00282843285671782</v>
       </c>
       <c r="J22" s="3" t="n">
         <f aca="false">AVERAGE(G22,E22,C22)</f>
-        <v>0.92961134004884</v>
-      </c>
-      <c r="K22" s="3" t="e">
+        <v>0.928371747176435</v>
+      </c>
+      <c r="K22" s="3" t="n">
         <f aca="false">STDEV(G22,E22,C22)</f>
-        <v>#DIV/0!</v>
+        <v>0.00175304905197663</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +1045,7 @@
       <selection pane="topLeft" activeCell="M33" activeCellId="0" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.37"/>

</xml_diff>